<commit_message>
Day 16 part 1
</commit_message>
<xml_diff>
--- a/Advent of Code-Tracking-2022.xlsx
+++ b/Advent of Code-Tracking-2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aforgiel\source\repos\AdventOfCode2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BECED70-2935-41A4-8C25-61D66E05E196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2943D1C4-F38E-465B-A4E6-1158DB56126C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{DFEEB8B9-5279-44FF-B8AD-25775064E720}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{DFEEB8B9-5279-44FF-B8AD-25775064E720}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracking" sheetId="1" r:id="rId1"/>
@@ -147,49 +147,49 @@
     <t xml:space="preserve"> 15   06:33:24   14233      0   07:46:22    9889      0</t>
   </si>
   <si>
-    <t>15   13522  6367  *****</t>
-  </si>
-  <si>
-    <t>14   31625   970  *******</t>
-  </si>
-  <si>
-    <t>13   35931  1000  ********</t>
-  </si>
-  <si>
-    <t>12   43165   811  *********</t>
-  </si>
-  <si>
-    <t>11   52814  7269  ***********</t>
-  </si>
-  <si>
-    <t>10   66628  4130  *************</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 9   65579  9050  **************</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 8   86299  6006  *****************</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 7   91897  1886  *****************</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 6  127452  1130  ***********************</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5  129301  2259  ***********************</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4  151362  2623  ***************************</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3  164068  8168  ******************************</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2  190432  8667  ***********************************</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1  227380  9638  *****************************************</t>
+    <t>15   14723  6476  *****</t>
+  </si>
+  <si>
+    <t>14   31857   946  *******</t>
+  </si>
+  <si>
+    <t>13   36069   995  ********</t>
+  </si>
+  <si>
+    <t>12   43255   803  *********</t>
+  </si>
+  <si>
+    <t>11   52911  7275  ***********</t>
+  </si>
+  <si>
+    <t>10   66722  4145  *************</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9   65655  9067  **************</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8   86398  5984  *****************</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7   91979  1894  *****************</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6  127547  1132  ***********************</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5  129392  2264  ***********************</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4  151468  2635  ***************************</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3  164192  8159  ******************************</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2  190564  8672  ***********************************</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1  227525  9636  *****************************************</t>
   </si>
 </sst>
 </file>
@@ -565,12 +565,12 @@
   <dimension ref="B2:N43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
     <col min="3" max="3" width="30.5703125" customWidth="1" outlineLevel="1"/>
     <col min="4" max="4" width="3.140625" customWidth="1" outlineLevel="1"/>
     <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1" outlineLevel="1"/>
@@ -956,7 +956,7 @@
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
-        <v>15 13522 6367 *****</v>
+        <v>15 14723 6476 *****</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="1"/>
@@ -972,19 +972,19 @@
       </c>
       <c r="K12" s="2">
         <f t="shared" si="3"/>
-        <v>6367</v>
+        <v>6476</v>
       </c>
       <c r="L12" s="2">
         <f t="shared" si="4"/>
-        <v>13522</v>
+        <v>14723</v>
       </c>
       <c r="M12" s="5">
         <f t="shared" si="8"/>
-        <v>-0.57242687747035581</v>
+        <v>-0.53784097686536714</v>
       </c>
       <c r="N12" s="4">
         <f t="shared" si="5"/>
-        <v>19889</v>
+        <v>21199</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
@@ -993,7 +993,7 @@
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
-        <v>14 31625 970 *******</v>
+        <v>14 31857 946 *******</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="1"/>
@@ -1009,19 +1009,19 @@
       </c>
       <c r="K13" s="2">
         <f t="shared" si="3"/>
-        <v>970</v>
+        <v>946</v>
       </c>
       <c r="L13" s="2">
         <f t="shared" si="4"/>
-        <v>31625</v>
+        <v>31857</v>
       </c>
       <c r="M13" s="5">
         <f t="shared" si="8"/>
-        <v>-0.11984080598925717</v>
+        <v>-0.1167761789902686</v>
       </c>
       <c r="N13" s="4">
         <f t="shared" si="5"/>
-        <v>32595</v>
+        <v>32803</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
@@ -1030,7 +1030,7 @@
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
-        <v>13 35931 1000 ********</v>
+        <v>13 36069 995 ********</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="1"/>
@@ -1042,23 +1042,23 @@
       </c>
       <c r="F14" s="2">
         <f t="shared" si="7"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K14" s="2">
         <f t="shared" si="3"/>
-        <v>1000</v>
+        <v>995</v>
       </c>
       <c r="L14" s="2">
         <f t="shared" si="4"/>
-        <v>35931</v>
+        <v>36069</v>
       </c>
       <c r="M14" s="5">
         <f t="shared" si="8"/>
-        <v>-0.16758948221939074</v>
+        <v>-0.16613108311177893</v>
       </c>
       <c r="N14" s="4">
         <f t="shared" si="5"/>
-        <v>36931</v>
+        <v>37064</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
@@ -1067,7 +1067,7 @@
       </c>
       <c r="C15" t="str">
         <f t="shared" ref="C15" si="20">TRIM(B15)</f>
-        <v>12 43165 811 *********</v>
+        <v>12 43255 803 *********</v>
       </c>
       <c r="D15" s="2">
         <f>FIND($D$28,$C15)</f>
@@ -1083,19 +1083,19 @@
       </c>
       <c r="K15" s="2">
         <f>VALUE(MID($C15,E15+1,F15-E15-1))</f>
-        <v>811</v>
+        <v>803</v>
       </c>
       <c r="L15" s="2">
         <f>VALUE(MID($C15,D15+1,E15-D15-1))</f>
-        <v>43165</v>
+        <v>43255</v>
       </c>
       <c r="M15" s="5">
         <f t="shared" si="8"/>
-        <v>-0.18269776953080619</v>
+        <v>-0.18249513333711331</v>
       </c>
       <c r="N15" s="4">
         <f t="shared" ref="N15" si="21">SUM(K15:L15)</f>
-        <v>43976</v>
+        <v>44058</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
@@ -1104,7 +1104,7 @@
       </c>
       <c r="C16" t="str">
         <f t="shared" ref="C16:C26" si="22">TRIM(B16)</f>
-        <v>11 52814 7269 ***********</v>
+        <v>11 52911 7275 ***********</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" ref="D16:D26" si="23">FIND($D$28,$C16)</f>
@@ -1120,19 +1120,19 @@
       </c>
       <c r="K16" s="2">
         <f t="shared" ref="K16:K26" si="25">VALUE(MID($C16,E16+1,F16-E16-1))</f>
-        <v>7269</v>
+        <v>7275</v>
       </c>
       <c r="L16" s="2">
         <f t="shared" ref="L16:L26" si="26">VALUE(MID($C16,D16+1,E16-D16-1))</f>
-        <v>52814</v>
+        <v>52911</v>
       </c>
       <c r="M16" s="5">
         <f t="shared" si="8"/>
-        <v>-0.20733025154589657</v>
+        <v>-0.20699319564761243</v>
       </c>
       <c r="N16" s="4">
         <f t="shared" ref="N16:N26" si="27">SUM(K16:L16)</f>
-        <v>60083</v>
+        <v>60186</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
@@ -1141,7 +1141,7 @@
       </c>
       <c r="C17" t="str">
         <f t="shared" si="22"/>
-        <v>10 66628 4130 *************</v>
+        <v>10 66722 4145 *************</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="23"/>
@@ -1157,19 +1157,19 @@
       </c>
       <c r="K17" s="2">
         <f t="shared" si="25"/>
-        <v>4130</v>
+        <v>4145</v>
       </c>
       <c r="L17" s="2">
         <f t="shared" si="26"/>
-        <v>66628</v>
+        <v>66722</v>
       </c>
       <c r="M17" s="5">
         <f t="shared" si="8"/>
-        <v>1.5995974321047823E-2</v>
+        <v>1.6251618307821181E-2</v>
       </c>
       <c r="N17" s="4">
         <f t="shared" si="27"/>
-        <v>70758</v>
+        <v>70867</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
@@ -1178,7 +1178,7 @@
       </c>
       <c r="C18" t="str">
         <f t="shared" si="22"/>
-        <v>9 65579 9050 **************</v>
+        <v>9 65655 9067 **************</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="23"/>
@@ -1194,19 +1194,19 @@
       </c>
       <c r="K18" s="2">
         <f t="shared" si="25"/>
-        <v>9050</v>
+        <v>9067</v>
       </c>
       <c r="L18" s="2">
         <f t="shared" si="26"/>
-        <v>65579</v>
+        <v>65655</v>
       </c>
       <c r="M18" s="5">
         <f t="shared" si="8"/>
-        <v>-0.240095481987045</v>
+        <v>-0.24008657607814998</v>
       </c>
       <c r="N18" s="4">
         <f t="shared" si="27"/>
-        <v>74629</v>
+        <v>74722</v>
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
@@ -1215,7 +1215,7 @@
       </c>
       <c r="C19" t="str">
         <f t="shared" si="22"/>
-        <v>8 86299 6006 *****************</v>
+        <v>8 86398 5984 *****************</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="23"/>
@@ -1231,19 +1231,19 @@
       </c>
       <c r="K19" s="2">
         <f t="shared" si="25"/>
-        <v>6006</v>
+        <v>5984</v>
       </c>
       <c r="L19" s="2">
         <f t="shared" si="26"/>
-        <v>86299</v>
+        <v>86398</v>
       </c>
       <c r="M19" s="5">
         <f t="shared" si="8"/>
-        <v>-6.0916025550344366E-2</v>
+        <v>-6.0676893638765383E-2</v>
       </c>
       <c r="N19" s="4">
         <f t="shared" si="27"/>
-        <v>92305</v>
+        <v>92382</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
@@ -1252,7 +1252,7 @@
       </c>
       <c r="C20" t="str">
         <f t="shared" si="22"/>
-        <v>7 91897 1886 *****************</v>
+        <v>7 91979 1894 *****************</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="23"/>
@@ -1268,19 +1268,19 @@
       </c>
       <c r="K20" s="2">
         <f t="shared" si="25"/>
-        <v>1886</v>
+        <v>1894</v>
       </c>
       <c r="L20" s="2">
         <f t="shared" si="26"/>
-        <v>91897</v>
+        <v>91979</v>
       </c>
       <c r="M20" s="5">
         <f t="shared" si="8"/>
-        <v>-0.27896776825785397</v>
+        <v>-0.27886190972739455</v>
       </c>
       <c r="N20" s="4">
         <f t="shared" si="27"/>
-        <v>93783</v>
+        <v>93873</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="C21" t="str">
         <f t="shared" si="22"/>
-        <v>6 127452 1130 ***********************</v>
+        <v>6 127547 1132 ***********************</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="23"/>
@@ -1305,19 +1305,19 @@
       </c>
       <c r="K21" s="2">
         <f t="shared" si="25"/>
-        <v>1130</v>
+        <v>1132</v>
       </c>
       <c r="L21" s="2">
         <f t="shared" si="26"/>
-        <v>127452</v>
+        <v>127547</v>
       </c>
       <c r="M21" s="5">
         <f t="shared" si="8"/>
-        <v>-1.429996674426337E-2</v>
+        <v>-1.4258995919376738E-2</v>
       </c>
       <c r="N21" s="4">
         <f t="shared" si="27"/>
-        <v>128582</v>
+        <v>128679</v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
@@ -1326,7 +1326,7 @@
       </c>
       <c r="C22" t="str">
         <f t="shared" si="22"/>
-        <v>5 129301 2259 ***********************</v>
+        <v>5 129392 2264 ***********************</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" si="23"/>
@@ -1342,19 +1342,19 @@
       </c>
       <c r="K22" s="2">
         <f t="shared" si="25"/>
-        <v>2259</v>
+        <v>2264</v>
       </c>
       <c r="L22" s="2">
         <f t="shared" si="26"/>
-        <v>129301</v>
+        <v>129392</v>
       </c>
       <c r="M22" s="5">
         <f t="shared" si="8"/>
-        <v>-0.14574992402320264</v>
+        <v>-0.14574695645284808</v>
       </c>
       <c r="N22" s="4">
         <f t="shared" si="27"/>
-        <v>131560</v>
+        <v>131656</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
@@ -1363,7 +1363,7 @@
       </c>
       <c r="C23" t="str">
         <f t="shared" si="22"/>
-        <v>4 151362 2623 ***************************</v>
+        <v>4 151468 2635 ***************************</v>
       </c>
       <c r="D23" s="2">
         <f t="shared" si="23"/>
@@ -1379,19 +1379,19 @@
       </c>
       <c r="K23" s="2">
         <f t="shared" si="25"/>
-        <v>2623</v>
+        <v>2635</v>
       </c>
       <c r="L23" s="2">
         <f t="shared" si="26"/>
-        <v>151362</v>
+        <v>151468</v>
       </c>
       <c r="M23" s="5">
         <f t="shared" si="8"/>
-        <v>-7.7443499036984664E-2</v>
+        <v>-7.749464042097054E-2</v>
       </c>
       <c r="N23" s="4">
         <f t="shared" si="27"/>
-        <v>153985</v>
+        <v>154103</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
@@ -1400,7 +1400,7 @@
       </c>
       <c r="C24" t="str">
         <f t="shared" si="22"/>
-        <v>3 164068 8168 ******************************</v>
+        <v>3 164192 8159 ******************************</v>
       </c>
       <c r="D24" s="2">
         <f t="shared" si="23"/>
@@ -1416,19 +1416,19 @@
       </c>
       <c r="K24" s="2">
         <f t="shared" si="25"/>
-        <v>8168</v>
+        <v>8159</v>
       </c>
       <c r="L24" s="2">
         <f t="shared" si="26"/>
-        <v>164068</v>
+        <v>164192</v>
       </c>
       <c r="M24" s="5">
         <f t="shared" si="8"/>
-        <v>-0.13844311880356241</v>
+        <v>-0.13838920257761167</v>
       </c>
       <c r="N24" s="4">
         <f t="shared" si="27"/>
-        <v>172236</v>
+        <v>172351</v>
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
@@ -1437,7 +1437,7 @@
       </c>
       <c r="C25" t="str">
         <f t="shared" si="22"/>
-        <v>2 190432 8667 ***********************************</v>
+        <v>2 190564 8672 ***********************************</v>
       </c>
       <c r="D25" s="2">
         <f t="shared" si="23"/>
@@ -1453,19 +1453,19 @@
       </c>
       <c r="K25" s="2">
         <f t="shared" si="25"/>
-        <v>8667</v>
+        <v>8672</v>
       </c>
       <c r="L25" s="2">
         <f t="shared" si="26"/>
-        <v>190432</v>
+        <v>190564</v>
       </c>
       <c r="M25" s="5">
         <f t="shared" si="8"/>
-        <v>-0.16249450259477527</v>
+        <v>-0.16244808262828259</v>
       </c>
       <c r="N25" s="4">
         <f t="shared" si="27"/>
-        <v>199099</v>
+        <v>199236</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
@@ -1474,7 +1474,7 @@
       </c>
       <c r="C26" t="str">
         <f t="shared" si="22"/>
-        <v>1 227380 9638 *****************************************</v>
+        <v>1 227525 9636 *****************************************</v>
       </c>
       <c r="D26" s="2">
         <f t="shared" si="23"/>
@@ -1490,15 +1490,15 @@
       </c>
       <c r="K26" s="2">
         <f t="shared" si="25"/>
-        <v>9638</v>
+        <v>9636</v>
       </c>
       <c r="L26" s="2">
         <f t="shared" si="26"/>
-        <v>227380</v>
+        <v>227525</v>
       </c>
       <c r="N26" s="4">
         <f t="shared" si="27"/>
-        <v>237018</v>
+        <v>237161</v>
       </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
@@ -1561,11 +1561,11 @@
       </c>
       <c r="M29" s="3" cm="1">
         <f t="array" ref="M29">L29/INDEX($N$2:$N$26,26-J29)</f>
-        <v>0.49720951279601788</v>
+        <v>0.46648426812585497</v>
       </c>
       <c r="N29" s="3">
         <f t="shared" ref="N29" si="44">L29/$N$26</f>
-        <v>4.1722569593870509E-2</v>
+        <v>4.1697412306407881E-2</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
@@ -1614,11 +1614,11 @@
       </c>
       <c r="M30" s="3" cm="1">
         <f t="array" ref="M30">L30/INDEX($N$2:$N$26,26-J30)</f>
-        <v>0.37389170118116277</v>
+        <v>0.37152089747888911</v>
       </c>
       <c r="N30" s="3">
         <f t="shared" ref="N30:N43" si="54">L30/$N$26</f>
-        <v>5.1418035760997058E-2</v>
+        <v>5.1387032437879752E-2</v>
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
@@ -1667,11 +1667,11 @@
       </c>
       <c r="M31" s="3" cm="1">
         <f t="array" ref="M31">L31/INDEX($N$2:$N$26,26-J31)</f>
-        <v>0.32606753134223282</v>
+        <v>0.32489747463846319</v>
       </c>
       <c r="N31" s="3">
         <f t="shared" si="54"/>
-        <v>5.0806267878388982E-2</v>
+        <v>5.0775633430454416E-2</v>
       </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
@@ -1720,11 +1720,11 @@
       </c>
       <c r="M32" s="3" cm="1">
         <f t="array" ref="M32">L32/INDEX($N$2:$N$26,26-J32)</f>
-        <v>0.3950336547207568</v>
+        <v>0.39429842480366789</v>
       </c>
       <c r="N32" s="3">
         <f t="shared" si="54"/>
-        <v>7.3294011425292599E-2</v>
+        <v>7.3249817634433986E-2</v>
       </c>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
@@ -1773,11 +1773,11 @@
       </c>
       <c r="M33" s="3" cm="1">
         <f t="array" ref="M33">L33/INDEX($N$2:$N$26,26-J33)</f>
-        <v>0.28811810329044824</v>
+        <v>0.28762502907652943</v>
       </c>
       <c r="N33" s="3">
         <f t="shared" si="54"/>
-        <v>7.3036647005712649E-2</v>
+        <v>7.2992608396827474E-2</v>
       </c>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
@@ -1826,11 +1826,11 @@
       </c>
       <c r="M34" s="3" cm="1">
         <f t="array" ref="M34">L34/INDEX($N$2:$N$26,26-J34)</f>
-        <v>0.58204019333502921</v>
+        <v>0.58114496168879737</v>
       </c>
       <c r="N34" s="3">
         <f t="shared" si="54"/>
-        <v>0.17375895501607472</v>
+        <v>0.17365418428831048</v>
       </c>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
@@ -1879,11 +1879,11 @@
       </c>
       <c r="M35" s="3" cm="1">
         <f t="array" ref="M35">L35/INDEX($N$2:$N$26,26-J35)</f>
-        <v>0.14180814428707339</v>
+        <v>0.14163164797516126</v>
       </c>
       <c r="N35" s="3">
         <f t="shared" si="54"/>
-        <v>4.4650617252698109E-2</v>
+        <v>4.4623694452291904E-2</v>
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.25">
@@ -1932,11 +1932,11 @@
       </c>
       <c r="M36" s="3" cm="1">
         <f t="array" ref="M36">L36/INDEX($N$2:$N$26,26-J36)</f>
-        <v>0.1753642814582092</v>
+        <v>0.17521811608321969</v>
       </c>
       <c r="N36" s="3">
         <f t="shared" si="54"/>
-        <v>6.8294391143288696E-2</v>
+        <v>6.8253211953061416E-2</v>
       </c>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
@@ -1985,11 +1985,11 @@
       </c>
       <c r="M37" s="3" cm="1">
         <f t="array" ref="M37">L37/INDEX($N$2:$N$26,26-J37)</f>
-        <v>0.20039879295821203</v>
+        <v>0.20020666219253672</v>
       </c>
       <c r="N37" s="3">
         <f t="shared" si="54"/>
-        <v>7.9293555763697274E-2</v>
+        <v>7.9245744452081074E-2</v>
       </c>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
@@ -2038,11 +2038,11 @@
       </c>
       <c r="M38" s="3" cm="1">
         <f t="array" ref="M38">L38/INDEX($N$2:$N$26,26-J38)</f>
-        <v>0.62694622886562656</v>
+        <v>0.62647362817553753</v>
       </c>
       <c r="N38" s="3">
         <f t="shared" si="54"/>
-        <v>0.34011762819701458</v>
+        <v>0.33991254885921379</v>
       </c>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
@@ -2091,11 +2091,11 @@
       </c>
       <c r="M39" s="3" cm="1">
         <f t="array" ref="M39">L39/INDEX($N$2:$N$26,26-J39)</f>
-        <v>0.73178017634539372</v>
+        <v>0.73124658200157988</v>
       </c>
       <c r="N39" s="3">
         <f t="shared" si="54"/>
-        <v>0.40618434042984075</v>
+        <v>0.40593942511627124</v>
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.25">
@@ -2144,11 +2144,11 @@
       </c>
       <c r="M40" s="3" cm="1">
         <f t="array" ref="M40">L40/INDEX($N$2:$N$26,26-J40)</f>
-        <v>0.77490664675130694</v>
+        <v>0.77431328397240806</v>
       </c>
       <c r="N40" s="3">
         <f t="shared" si="54"/>
-        <v>0.5034385574091419</v>
+        <v>0.50313500111738441</v>
       </c>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.25">
@@ -2197,11 +2197,11 @@
       </c>
       <c r="M41" s="3" cm="1">
         <f t="array" ref="M41">L41/INDEX($N$2:$N$26,26-J41)</f>
-        <v>0.76388792122436655</v>
+        <v>0.76337822234857933</v>
       </c>
       <c r="N41" s="3">
         <f t="shared" si="54"/>
-        <v>0.55510130032318217</v>
+        <v>0.55476659315823429</v>
       </c>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
@@ -2250,11 +2250,11 @@
       </c>
       <c r="M42" s="3" cm="1">
         <f t="array" ref="M42">L42/INDEX($N$2:$N$26,26-J42)</f>
-        <v>0.79332894690581068</v>
+        <v>0.79278343271296348</v>
       </c>
       <c r="N42" s="3">
         <f t="shared" si="54"/>
-        <v>0.66640930224708672</v>
+        <v>0.66600748015061495</v>
       </c>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.25">
@@ -2303,11 +2303,11 @@
       </c>
       <c r="M43" s="3" cm="1">
         <f t="array" ref="M43">L43/INDEX($N$2:$N$26,26-J43)</f>
-        <v>0.80929296509125892</v>
+        <v>0.80880498901590059</v>
       </c>
       <c r="N43" s="3">
         <f t="shared" si="54"/>
-        <v>0.80929296509125892</v>
+        <v>0.80880498901590059</v>
       </c>
     </row>
   </sheetData>

</xml_diff>